<commit_message>
[ML] Change calculation of diff_mean to difference in means between the 'fake' and 'other' classes for each feature, where the data points for each feature are scaled to mean of 0 and standard deviation of 1. This allows diff_mean to be a reasonable metric which can be compared among different features.
</commit_message>
<xml_diff>
--- a/statistics.xlsx
+++ b/statistics.xlsx
@@ -85,25 +85,25 @@
     <t>user_name_has_nonprintable_chars</t>
   </si>
   <si>
+    <t>user_name_has_weird_chars</t>
+  </si>
+  <si>
+    <t>num_mentions_is_more_than_2</t>
+  </si>
+  <si>
+    <t>user_name_num_digits_underscores</t>
+  </si>
+  <si>
+    <t>num_urls</t>
+  </si>
+  <si>
+    <t>num_urls_is_nonzero</t>
+  </si>
+  <si>
+    <t>user_favourites_count</t>
+  </si>
+  <si>
     <t>user_name_num_nonprintable_chars</t>
-  </si>
-  <si>
-    <t>user_name_has_weird_chars</t>
-  </si>
-  <si>
-    <t>num_mentions_is_more_than_2</t>
-  </si>
-  <si>
-    <t>user_name_num_digits_underscores</t>
-  </si>
-  <si>
-    <t>num_urls</t>
-  </si>
-  <si>
-    <t>num_urls_is_nonzero</t>
-  </si>
-  <si>
-    <t>user_favourites_count</t>
   </si>
   <si>
     <t>user_name_num_underscores</t>
@@ -418,145 +418,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB3AFE4"/>
+        <fgColor rgb="FFBDA6E4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF8DFC2"/>
+        <fgColor rgb="FFFDE2CD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA49AAB"/>
+        <fgColor rgb="FFA7CDE4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEDDAA9"/>
+        <fgColor rgb="FFDED9D5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC0B2FD"/>
+        <fgColor rgb="FFD5FEF4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA696B4"/>
+        <fgColor rgb="FFB397B9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDBDBD9"/>
+        <fgColor rgb="FFC5A4FD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE4C9DB"/>
+        <fgColor rgb="FFEFA8CC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA7D1B5"/>
+        <fgColor rgb="FFB8BFEA"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE49A97"/>
+        <fgColor rgb="FF99DBA8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFBBE4BD"/>
+        <fgColor rgb="FFDCADFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA8C3A8"/>
+        <fgColor rgb="FFB3AFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF6EEAD"/>
+        <fgColor rgb="FFDCDCE2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD3A4A6"/>
+        <fgColor rgb="FFACDECD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC3BDF0"/>
+        <fgColor rgb="FF9DD7F8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB1B5E1"/>
+        <fgColor rgb="FFF5B3B7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDCCACC"/>
+        <fgColor rgb="FFB0DB96"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA4E8D3"/>
+        <fgColor rgb="FFE4F3D4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF7FCBE"/>
+        <fgColor rgb="FFC7C697"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE2DAC4"/>
+        <fgColor rgb="FFC3DBE1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCE96A5"/>
+        <fgColor rgb="FFFEDBC2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCBA3F8"/>
+        <fgColor rgb="FFBA999F"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCEECB1"/>
+        <fgColor rgb="FFC0DDB7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD8B4D6"/>
+        <fgColor rgb="FF9CDC9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1073,16 +1073,16 @@
         <v>8</v>
       </c>
       <c r="B5" s="12">
-        <v>1.866997261035956</v>
+        <v>1.843557631086175</v>
       </c>
       <c r="C5" s="12">
-        <v>0.5158126067704628</v>
+        <v>0.5157993155584074</v>
       </c>
       <c r="D5" s="13">
-        <v>0.0007812871834360839</v>
+        <v>0.0008037934770308429</v>
       </c>
       <c r="E5" s="12">
-        <v>3.361092500038028</v>
+        <v>3.35322549038706</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1158,16 +1158,16 @@
         <v>13</v>
       </c>
       <c r="B10" s="24">
-        <v>-454.9451879020083</v>
+        <v>-450.2063900838606</v>
       </c>
       <c r="C10" s="24">
-        <v>-0.3933589370694147</v>
+        <v>-0.392095559812901</v>
       </c>
       <c r="D10" s="25">
-        <v>0.0002767655536177508</v>
+        <v>0.0002528630914822416</v>
       </c>
       <c r="E10" s="24">
-        <v>-3.638324509313828</v>
+        <v>-3.661578251382192</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1243,16 +1243,16 @@
         <v>18</v>
       </c>
       <c r="B15" s="30">
-        <v>2.109169134335639</v>
+        <v>2.087708493567302</v>
       </c>
       <c r="C15" s="30">
-        <v>0.3267733610768643</v>
+        <v>0.3268044343797739</v>
       </c>
       <c r="D15" s="31">
-        <v>0.01064188111794005</v>
+        <v>0.01063613429788991</v>
       </c>
       <c r="E15" s="30">
-        <v>2.555059177323764</v>
+        <v>2.555247401007956</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1328,118 +1328,118 @@
         <v>23</v>
       </c>
       <c r="B20" s="15">
-        <v>0.01529258298269268</v>
+        <v>0.02813662154841286</v>
       </c>
       <c r="C20" s="15">
-        <v>0.2870524971337281</v>
+        <v>0.2864201164185585</v>
       </c>
       <c r="D20" s="16">
-        <v>0.07878999542386135</v>
+        <v>0.01466390719685074</v>
       </c>
       <c r="E20" s="15">
-        <v>1.758055427361527</v>
+        <v>2.441295409585917</v>
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="15">
-        <v>0.02813662154841286</v>
-      </c>
-      <c r="C21" s="15">
-        <v>0.2864201164185585</v>
-      </c>
-      <c r="D21" s="16">
-        <v>0.01466390719685074</v>
-      </c>
-      <c r="E21" s="15">
-        <v>2.441295409585917</v>
+      <c r="B21" s="42">
+        <v>0.009268725840417429</v>
+      </c>
+      <c r="C21" s="42">
+        <v>0.2860202623215724</v>
+      </c>
+      <c r="D21" s="43">
+        <v>0.1766642497996158</v>
+      </c>
+      <c r="E21" s="42">
+        <v>1.35125934836063</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="42">
-        <v>0.009268725840417429</v>
-      </c>
-      <c r="C22" s="42">
-        <v>0.2860202623215724</v>
-      </c>
-      <c r="D22" s="43">
-        <v>0.1766642497996158</v>
-      </c>
-      <c r="E22" s="42">
-        <v>1.35125934836063</v>
+      <c r="B22" s="15">
+        <v>0.03043903740483823</v>
+      </c>
+      <c r="C22" s="15">
+        <v>0.2570310694328317</v>
+      </c>
+      <c r="D22" s="16">
+        <v>0.2608058985485498</v>
+      </c>
+      <c r="E22" s="15">
+        <v>1.124596431394523</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="15">
-        <v>0.03043903740483823</v>
-      </c>
-      <c r="C23" s="15">
-        <v>0.2570310694328317</v>
-      </c>
-      <c r="D23" s="16">
-        <v>0.2608058985485498</v>
-      </c>
-      <c r="E23" s="15">
-        <v>1.124596431394523</v>
+      <c r="B23" s="45">
+        <v>0.09513631197989431</v>
+      </c>
+      <c r="C23" s="45">
+        <v>0.250775233814623</v>
+      </c>
+      <c r="D23" s="46">
+        <v>6.345772471463819e-07</v>
+      </c>
+      <c r="E23" s="45">
+        <v>4.985843688342034</v>
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="44" t="s">
+      <c r="A24" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="45">
-        <v>0.09513631197989431</v>
-      </c>
-      <c r="C24" s="45">
-        <v>0.250775233814623</v>
-      </c>
-      <c r="D24" s="46">
-        <v>6.345772471463819e-07</v>
-      </c>
-      <c r="E24" s="45">
-        <v>4.985843688342034</v>
+      <c r="B24" s="48">
+        <v>0.0938145358712521</v>
+      </c>
+      <c r="C24" s="48">
+        <v>0.2499741746949186</v>
+      </c>
+      <c r="D24" s="49">
+        <v>5.554662670952748e-07</v>
+      </c>
+      <c r="E24" s="48">
+        <v>5.011631522099299</v>
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="47" t="s">
+      <c r="A25" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="48">
-        <v>0.0938145358712521</v>
-      </c>
-      <c r="C25" s="48">
-        <v>0.2499741746949186</v>
-      </c>
-      <c r="D25" s="49">
-        <v>5.554662670952748e-07</v>
-      </c>
-      <c r="E25" s="48">
-        <v>5.011631522099299</v>
+      <c r="B25" s="30">
+        <v>2824.184266078215</v>
+      </c>
+      <c r="C25" s="30">
+        <v>0.2428288211068139</v>
+      </c>
+      <c r="D25" s="31">
+        <v>0.07899865235454698</v>
+      </c>
+      <c r="E25" s="30">
+        <v>1.756830440596375</v>
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="30">
-        <v>2824.184266078215</v>
-      </c>
-      <c r="C26" s="30">
-        <v>0.2428288211068139</v>
-      </c>
-      <c r="D26" s="31">
-        <v>0.07899865235454698</v>
-      </c>
-      <c r="E26" s="30">
-        <v>1.756830440596375</v>
+      <c r="B26" s="15">
+        <v>0.0591881769265549</v>
+      </c>
+      <c r="C26" s="15">
+        <v>0.2330361488344119</v>
+      </c>
+      <c r="D26" s="16">
+        <v>0.28097418974511</v>
+      </c>
+      <c r="E26" s="15">
+        <v>1.078232414300121</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1464,16 +1464,16 @@
         <v>31</v>
       </c>
       <c r="B28" s="51">
-        <v>-0.8728037331538636</v>
+        <v>-0.8667094347112938</v>
       </c>
       <c r="C28" s="51">
-        <v>-0.2210862031281594</v>
+        <v>-0.2206850842391159</v>
       </c>
       <c r="D28" s="52">
-        <v>0.0006400100521255085</v>
+        <v>0.0006598264203504922</v>
       </c>
       <c r="E28" s="51">
-        <v>-3.415900494743193</v>
+        <v>-3.407571252368454</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1634,16 +1634,16 @@
         <v>41</v>
       </c>
       <c r="B38" s="63">
-        <v>3.054585974784404</v>
+        <v>3.021404385478446</v>
       </c>
       <c r="C38" s="63">
-        <v>0.194714156560507</v>
+        <v>0.1939584297157631</v>
       </c>
       <c r="D38" s="64">
-        <v>0.002687569742260673</v>
+        <v>0.002800949297166008</v>
       </c>
       <c r="E38" s="63">
-        <v>3.002657286108902</v>
+        <v>2.990038808446408</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1923,16 +1923,16 @@
         <v>58</v>
       </c>
       <c r="B55" s="87">
-        <v>0.2180610229925666</v>
+        <v>0.2050754445073215</v>
       </c>
       <c r="C55" s="87">
-        <v>0.09597278456914227</v>
+        <v>0.09216925896422574</v>
       </c>
       <c r="D55" s="88">
-        <v>0.4792362261483942</v>
+        <v>0.4839225858035684</v>
       </c>
       <c r="E55" s="87">
-        <v>0.7075765814223602</v>
+        <v>0.7000518140404699</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -2212,16 +2212,16 @@
         <v>75</v>
       </c>
       <c r="B72" s="108">
-        <v>-73.46274281780688</v>
+        <v>-73.4625223520693</v>
       </c>
       <c r="C72" s="108">
-        <v>-0.03041428900843226</v>
+        <v>-0.03026571770502225</v>
       </c>
       <c r="D72" s="109">
-        <v>0.04353423148663659</v>
+        <v>0.04353385496254215</v>
       </c>
       <c r="E72" s="108">
-        <v>-2.018982607954483</v>
+        <v>-2.018986229318218</v>
       </c>
     </row>
     <row r="73" spans="1:5">

</xml_diff>